<commit_message>
fixed motion planning fail
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point_motion.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point_motion.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.251</v>
+        <v>-0.157</v>
       </c>
       <c r="B1" t="n">
-        <v>0.113</v>
+        <v>-0.33</v>
       </c>
       <c r="C1" t="n">
-        <v>0.199</v>
+        <v>-0.033</v>
       </c>
       <c r="D1" t="n">
-        <v>-173</v>
+        <v>-116</v>
       </c>
       <c r="E1" t="n">
-        <v>-59</v>
+        <v>81</v>
       </c>
       <c r="F1" t="n">
-        <v>-147</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.059</v>
+        <v>0.103</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.08699999999999999</v>
+        <v>0.168</v>
       </c>
       <c r="C2" t="n">
-        <v>0.203</v>
+        <v>-0.09</v>
       </c>
       <c r="D2" t="n">
-        <v>-79</v>
+        <v>157</v>
       </c>
       <c r="E2" t="n">
-        <v>27</v>
+        <v>-35</v>
       </c>
       <c r="F2" t="n">
-        <v>-99</v>
+        <v>-168</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.113</v>
+        <v>0.117</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.03</v>
+        <v>-0.025</v>
       </c>
       <c r="C3" t="n">
-        <v>0.225</v>
+        <v>0.472</v>
       </c>
       <c r="D3" t="n">
-        <v>82</v>
+        <v>-179</v>
       </c>
       <c r="E3" t="n">
-        <v>-10</v>
+        <v>68</v>
       </c>
       <c r="F3" t="n">
-        <v>176</v>
+        <v>-71</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.05</v>
+        <v>0.303</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.046</v>
+        <v>-0.213</v>
       </c>
       <c r="C4" t="n">
-        <v>0.383</v>
+        <v>0.294</v>
       </c>
       <c r="D4" t="n">
-        <v>-168</v>
+        <v>21</v>
       </c>
       <c r="E4" t="n">
-        <v>-47</v>
+        <v>46</v>
       </c>
       <c r="F4" t="n">
-        <v>66</v>
+        <v>-69</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.065</v>
+        <v>-0.23</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.06</v>
+        <v>-0.194</v>
       </c>
       <c r="C5" t="n">
-        <v>0.254</v>
+        <v>0.006</v>
       </c>
       <c r="D5" t="n">
-        <v>71</v>
+        <v>-135</v>
       </c>
       <c r="E5" t="n">
-        <v>-53</v>
+        <v>29</v>
       </c>
       <c r="F5" t="n">
-        <v>-61</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.256</v>
+        <v>0.247</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.168</v>
+        <v>0.214</v>
       </c>
       <c r="C6" t="n">
-        <v>0.238</v>
+        <v>0.504</v>
       </c>
       <c r="D6" t="n">
-        <v>161</v>
+        <v>95</v>
       </c>
       <c r="E6" t="n">
-        <v>-13</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
-        <v>-140</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.145</v>
+        <v>0.066</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.096</v>
+        <v>-0.212</v>
       </c>
       <c r="C7" t="n">
-        <v>0.413</v>
+        <v>0.275</v>
       </c>
       <c r="D7" t="n">
-        <v>-83</v>
+        <v>-71</v>
       </c>
       <c r="E7" t="n">
-        <v>30</v>
+        <v>-63</v>
       </c>
       <c r="F7" t="n">
-        <v>-126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.204</v>
+        <v>-0.107</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.186</v>
+        <v>-0.445</v>
       </c>
       <c r="C8" t="n">
-        <v>0.13</v>
+        <v>-0.142</v>
       </c>
       <c r="D8" t="n">
-        <v>60</v>
+        <v>-73</v>
       </c>
       <c r="E8" t="n">
-        <v>-38</v>
+        <v>-42</v>
       </c>
       <c r="F8" t="n">
-        <v>-47</v>
+        <v>-176</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.021</v>
+        <v>0.134</v>
       </c>
       <c r="B9" t="n">
-        <v>0.127</v>
+        <v>0.232</v>
       </c>
       <c r="C9" t="n">
-        <v>0.115</v>
+        <v>0.182</v>
       </c>
       <c r="D9" t="n">
-        <v>-4</v>
+        <v>74</v>
       </c>
       <c r="E9" t="n">
-        <v>-13</v>
+        <v>38</v>
       </c>
       <c r="F9" t="n">
-        <v>-133</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.197</v>
+        <v>-0.287</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.103</v>
+        <v>-0.418</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.078</v>
+        <v>0.003</v>
       </c>
       <c r="D10" t="n">
-        <v>-128</v>
+        <v>-166</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
-        <v>-118</v>
+        <v>-109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
server train case 3
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point_motion.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point_motion.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-0.157</v>
+        <v>0.207</v>
       </c>
       <c r="B1" t="n">
-        <v>-0.33</v>
+        <v>0.372</v>
       </c>
       <c r="C1" t="n">
-        <v>-0.033</v>
+        <v>0.245</v>
       </c>
       <c r="D1" t="n">
-        <v>-116</v>
+        <v>-19</v>
       </c>
       <c r="E1" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" t="n">
-        <v>42</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.103</v>
+        <v>0.112</v>
       </c>
       <c r="B2" t="n">
-        <v>0.168</v>
+        <v>-0.118</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.09</v>
+        <v>0.473</v>
       </c>
       <c r="D2" t="n">
-        <v>157</v>
+        <v>74</v>
       </c>
       <c r="E2" t="n">
-        <v>-35</v>
+        <v>33</v>
       </c>
       <c r="F2" t="n">
-        <v>-168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.117</v>
+        <v>-0.001</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.025</v>
+        <v>0.224</v>
       </c>
       <c r="C3" t="n">
-        <v>0.472</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>-179</v>
+        <v>-56</v>
       </c>
       <c r="E3" t="n">
-        <v>68</v>
+        <v>-60</v>
       </c>
       <c r="F3" t="n">
-        <v>-71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.303</v>
+        <v>-0.174</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.213</v>
+        <v>-0.015</v>
       </c>
       <c r="C4" t="n">
-        <v>0.294</v>
+        <v>0.283</v>
       </c>
       <c r="D4" t="n">
-        <v>21</v>
+        <v>-20</v>
       </c>
       <c r="E4" t="n">
-        <v>46</v>
+        <v>-12</v>
       </c>
       <c r="F4" t="n">
-        <v>-69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.23</v>
+        <v>-0.081</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.194</v>
+        <v>-0.034</v>
       </c>
       <c r="C5" t="n">
-        <v>0.006</v>
+        <v>0.11</v>
       </c>
       <c r="D5" t="n">
-        <v>-135</v>
+        <v>-71</v>
       </c>
       <c r="E5" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>7</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.247</v>
+        <v>0.003</v>
       </c>
       <c r="B6" t="n">
-        <v>0.214</v>
+        <v>0.101</v>
       </c>
       <c r="C6" t="n">
-        <v>0.504</v>
+        <v>0.265</v>
       </c>
       <c r="D6" t="n">
-        <v>95</v>
+        <v>-168</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="F6" t="n">
-        <v>175</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.066</v>
+        <v>0.212</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.212</v>
+        <v>0.089</v>
       </c>
       <c r="C7" t="n">
-        <v>0.275</v>
+        <v>0.197</v>
       </c>
       <c r="D7" t="n">
-        <v>-71</v>
+        <v>-11</v>
       </c>
       <c r="E7" t="n">
-        <v>-63</v>
+        <v>-20</v>
       </c>
       <c r="F7" t="n">
-        <v>124</v>
+        <v>-110</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.107</v>
+        <v>0.02</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.445</v>
+        <v>0.032</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.142</v>
+        <v>0.263</v>
       </c>
       <c r="D8" t="n">
-        <v>-73</v>
+        <v>107</v>
       </c>
       <c r="E8" t="n">
-        <v>-42</v>
+        <v>-80</v>
       </c>
       <c r="F8" t="n">
-        <v>-176</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.134</v>
+        <v>0.042</v>
       </c>
       <c r="B9" t="n">
-        <v>0.232</v>
+        <v>0.177</v>
       </c>
       <c r="C9" t="n">
-        <v>0.182</v>
+        <v>0.089</v>
       </c>
       <c r="D9" t="n">
-        <v>74</v>
+        <v>-75</v>
       </c>
       <c r="E9" t="n">
-        <v>38</v>
+        <v>-70</v>
       </c>
       <c r="F9" t="n">
-        <v>56</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.287</v>
+        <v>0.04</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.418</v>
+        <v>0.144</v>
       </c>
       <c r="C10" t="n">
-        <v>0.003</v>
+        <v>0.284</v>
       </c>
       <c r="D10" t="n">
-        <v>-166</v>
+        <v>172</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
+        <v>-5</v>
       </c>
       <c r="F10" t="n">
-        <v>-109</v>
+        <v>-30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed case3 obstacle random problem
</commit_message>
<xml_diff>
--- a/dynamics/src/dynamics/xlsx/task_point_motion.xlsx
+++ b/dynamics/src/dynamics/xlsx/task_point_motion.xlsx
@@ -423,202 +423,202 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0.207</v>
+        <v>0.274</v>
       </c>
       <c r="B1" t="n">
-        <v>0.372</v>
+        <v>0.601</v>
       </c>
       <c r="C1" t="n">
-        <v>0.245</v>
+        <v>0.471</v>
       </c>
       <c r="D1" t="n">
-        <v>-19</v>
+        <v>-82</v>
       </c>
       <c r="E1" t="n">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="F1" t="n">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.112</v>
+        <v>0.323</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.118</v>
+        <v>0.361</v>
       </c>
       <c r="C2" t="n">
-        <v>0.473</v>
+        <v>0.955</v>
       </c>
       <c r="D2" t="n">
-        <v>74</v>
+        <v>-126</v>
       </c>
       <c r="E2" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>166</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.001</v>
+        <v>-0.076</v>
       </c>
       <c r="B3" t="n">
-        <v>0.224</v>
+        <v>-0.317</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.499</v>
       </c>
       <c r="D3" t="n">
-        <v>-56</v>
+        <v>-42</v>
       </c>
       <c r="E3" t="n">
-        <v>-60</v>
+        <v>28</v>
       </c>
       <c r="F3" t="n">
-        <v>62</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.174</v>
+        <v>0.029</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.015</v>
+        <v>0.194</v>
       </c>
       <c r="C4" t="n">
-        <v>0.283</v>
+        <v>0.108</v>
       </c>
       <c r="D4" t="n">
-        <v>-20</v>
+        <v>87</v>
       </c>
       <c r="E4" t="n">
-        <v>-12</v>
+        <v>-28</v>
       </c>
       <c r="F4" t="n">
-        <v>98</v>
+        <v>-84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.081</v>
+        <v>0.04</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.034</v>
+        <v>-0.184</v>
       </c>
       <c r="C5" t="n">
-        <v>0.11</v>
+        <v>0.331</v>
       </c>
       <c r="D5" t="n">
-        <v>-71</v>
+        <v>-77</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="F5" t="n">
-        <v>-150</v>
+        <v>-129</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.003</v>
+        <v>0.25</v>
       </c>
       <c r="B6" t="n">
-        <v>0.101</v>
+        <v>-0.461</v>
       </c>
       <c r="C6" t="n">
-        <v>0.265</v>
+        <v>0.286</v>
       </c>
       <c r="D6" t="n">
-        <v>-168</v>
+        <v>76</v>
       </c>
       <c r="E6" t="n">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="F6" t="n">
-        <v>-4</v>
+        <v>-87</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.212</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="B7" t="n">
-        <v>0.089</v>
+        <v>-0.228</v>
       </c>
       <c r="C7" t="n">
-        <v>0.197</v>
+        <v>0.027</v>
       </c>
       <c r="D7" t="n">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="E7" t="n">
-        <v>-20</v>
+        <v>-45</v>
       </c>
       <c r="F7" t="n">
-        <v>-110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.02</v>
+        <v>-0.149</v>
       </c>
       <c r="B8" t="n">
-        <v>0.032</v>
+        <v>0.178</v>
       </c>
       <c r="C8" t="n">
-        <v>0.263</v>
+        <v>0.671</v>
       </c>
       <c r="D8" t="n">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="E8" t="n">
-        <v>-80</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-70</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.042</v>
+        <v>0.747</v>
       </c>
       <c r="B9" t="n">
-        <v>0.177</v>
+        <v>-0.077</v>
       </c>
       <c r="C9" t="n">
-        <v>0.089</v>
+        <v>0.675</v>
       </c>
       <c r="D9" t="n">
-        <v>-75</v>
+        <v>53</v>
       </c>
       <c r="E9" t="n">
-        <v>-70</v>
+        <v>25</v>
       </c>
       <c r="F9" t="n">
-        <v>-43</v>
+        <v>-160</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.04</v>
+        <v>-0.092</v>
       </c>
       <c r="B10" t="n">
-        <v>0.144</v>
+        <v>0.048</v>
       </c>
       <c r="C10" t="n">
-        <v>0.284</v>
+        <v>0.436</v>
       </c>
       <c r="D10" t="n">
-        <v>172</v>
+        <v>-51</v>
       </c>
       <c r="E10" t="n">
-        <v>-5</v>
+        <v>-54</v>
       </c>
       <c r="F10" t="n">
-        <v>-30</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>